<commit_message>
add factor for state purchases
</commit_message>
<xml_diff>
--- a/results/12-2020/fim_interactive.xlsx
+++ b/results/12-2020/fim_interactive.xlsx
@@ -3221,16 +3221,16 @@
         <v>1</v>
       </c>
       <c r="E87">
-        <v>3.274442939439371</v>
+        <v>6.807648377777404</v>
       </c>
       <c r="F87">
-        <v>4.485867473255149</v>
+        <v>5.369168832839658</v>
       </c>
       <c r="G87">
         <v>3.100508840408109</v>
       </c>
       <c r="H87">
-        <v>-3.368956404567739</v>
+        <v>0.1642490337702944</v>
       </c>
       <c r="I87">
         <v>3.542890503599001</v>
@@ -3251,16 +3251,16 @@
         <v>1</v>
       </c>
       <c r="E88">
-        <v>-2.987287850227718</v>
+        <v>-3.020017250891981</v>
       </c>
       <c r="F88">
-        <v>0.1666011145068151</v>
+        <v>1.041720123925258</v>
       </c>
       <c r="G88">
         <v>-0.7037459759121391</v>
       </c>
       <c r="H88">
-        <v>0.2868626796071934</v>
+        <v>0.2541332789429298</v>
       </c>
       <c r="I88">
         <v>-2.570404553922772</v>
@@ -3281,16 +3281,16 @@
         <v>1</v>
       </c>
       <c r="E89">
-        <v>-2.924166013534065</v>
+        <v>-2.956577902985297</v>
       </c>
       <c r="F89">
-        <v>-1.486200667880462</v>
+        <v>-0.6191846308248271</v>
       </c>
       <c r="G89">
         <v>-0.1499749553841785</v>
       </c>
       <c r="H89">
-        <v>-0.1256411816786448</v>
+        <v>-0.1580530711298772</v>
       </c>
       <c r="I89">
         <v>-2.648549876471242</v>
@@ -3311,16 +3311,16 @@
         <v>1</v>
       </c>
       <c r="E90">
-        <v>-2.597578075119432</v>
+        <v>-5.994976992591383</v>
       </c>
       <c r="F90">
-        <v>-1.308647249860461</v>
+        <v>-1.290980942172814</v>
       </c>
       <c r="G90">
         <v>-3.554553272110574</v>
       </c>
       <c r="H90">
-        <v>3.433091938529865</v>
+        <v>0.03569302105791428</v>
       </c>
       <c r="I90">
         <v>-2.476116741538723</v>
@@ -3344,7 +3344,7 @@
         <v>-6.368117040881671</v>
       </c>
       <c r="F91">
-        <v>-3.719287244940721</v>
+        <v>-4.584922296837583</v>
       </c>
       <c r="G91">
         <v>-0.148166807756484</v>
@@ -3374,7 +3374,7 @@
         <v>-1.976178782683645</v>
       </c>
       <c r="F92">
-        <v>-3.466509978054704</v>
+        <v>-4.323962679785499</v>
       </c>
       <c r="G92">
         <v>-0.04498415407605297</v>
@@ -3404,7 +3404,7 @@
         <v>-0.5269966399726116</v>
       </c>
       <c r="F93">
-        <v>-2.867217634664341</v>
+        <v>-3.716567364032327</v>
       </c>
       <c r="G93">
         <v>-0.0217634055200784</v>

</xml_diff>